<commit_message>
Reports included, fixed login screen
</commit_message>
<xml_diff>
--- a/Delivered/Inception/ProjectPlanRevised.xlsx
+++ b/Delivered/Inception/ProjectPlanRevised.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CAPSTONE\Inception\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CAPSTONE\Delivered\Inception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF23A195-89CF-4501-984B-F1A19634A169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB42DA5B-1A35-4561-8831-0D0B2C230297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$75</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$76</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -451,7 +451,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="209">
   <si>
     <t>WBS</t>
   </si>
@@ -1624,9 +1624,6 @@
     <t>Agile Iteration Summary</t>
   </si>
   <si>
-    <t>Unit Tests Plan and Results</t>
-  </si>
-  <si>
     <t>Transition</t>
   </si>
   <si>
@@ -1733,6 +1730,12 @@
   </si>
   <si>
     <t>Store/Product page code demonstration</t>
+  </si>
+  <si>
+    <t>Unit Tests Plan and Results - Admin</t>
+  </si>
+  <si>
+    <t>Unit Tests Plan and Results - User</t>
   </si>
 </sst>
 </file>
@@ -2178,7 +2181,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2314,6 +2317,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2643,7 +2652,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -3009,12 +3018,14 @@
     <xf numFmtId="0" fontId="42" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3025,21 +3036,22 @@
     <xf numFmtId="0" fontId="49" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3905,11 +3917,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CI75"/>
+  <dimension ref="A1:CI76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3939,7 +3951,7 @@
   <sheetData>
     <row r="1" spans="1:87" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="105" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -3947,29 +3959,29 @@
       <c r="E1" s="43"/>
       <c r="F1" s="43"/>
       <c r="I1" s="110"/>
-      <c r="K1" s="150" t="s">
+      <c r="K1" s="156" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="150"/>
-      <c r="M1" s="150"/>
-      <c r="N1" s="150"/>
-      <c r="O1" s="150"/>
-      <c r="P1" s="150"/>
-      <c r="Q1" s="150"/>
-      <c r="R1" s="150"/>
-      <c r="S1" s="150"/>
-      <c r="T1" s="150"/>
-      <c r="U1" s="150"/>
-      <c r="V1" s="150"/>
-      <c r="W1" s="150"/>
-      <c r="X1" s="150"/>
-      <c r="Y1" s="150"/>
-      <c r="Z1" s="150"/>
-      <c r="AA1" s="150"/>
-      <c r="AB1" s="150"/>
-      <c r="AC1" s="150"/>
-      <c r="AD1" s="150"/>
-      <c r="AE1" s="150"/>
+      <c r="L1" s="156"/>
+      <c r="M1" s="156"/>
+      <c r="N1" s="156"/>
+      <c r="O1" s="156"/>
+      <c r="P1" s="156"/>
+      <c r="Q1" s="156"/>
+      <c r="R1" s="156"/>
+      <c r="S1" s="156"/>
+      <c r="T1" s="156"/>
+      <c r="U1" s="156"/>
+      <c r="V1" s="156"/>
+      <c r="W1" s="156"/>
+      <c r="X1" s="156"/>
+      <c r="Y1" s="156"/>
+      <c r="Z1" s="156"/>
+      <c r="AA1" s="156"/>
+      <c r="AB1" s="156"/>
+      <c r="AC1" s="156"/>
+      <c r="AD1" s="156"/>
+      <c r="AE1" s="156"/>
     </row>
     <row r="2" spans="1:87" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
@@ -4014,11 +4026,11 @@
       <c r="B4" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="155">
+      <c r="C4" s="158">
         <v>43850</v>
       </c>
-      <c r="D4" s="155"/>
-      <c r="E4" s="155"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
       <c r="F4" s="91"/>
       <c r="G4" s="94" t="s">
         <v>68</v>
@@ -4028,240 +4040,240 @@
       </c>
       <c r="I4" s="92"/>
       <c r="J4" s="46"/>
-      <c r="K4" s="152" t="str">
+      <c r="K4" s="153" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="L4" s="153"/>
-      <c r="M4" s="153"/>
-      <c r="N4" s="153"/>
-      <c r="O4" s="153"/>
-      <c r="P4" s="153"/>
-      <c r="Q4" s="154"/>
-      <c r="R4" s="152" t="str">
+      <c r="L4" s="154"/>
+      <c r="M4" s="154"/>
+      <c r="N4" s="154"/>
+      <c r="O4" s="154"/>
+      <c r="P4" s="154"/>
+      <c r="Q4" s="155"/>
+      <c r="R4" s="153" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="S4" s="153"/>
-      <c r="T4" s="153"/>
-      <c r="U4" s="153"/>
-      <c r="V4" s="153"/>
-      <c r="W4" s="153"/>
-      <c r="X4" s="154"/>
-      <c r="Y4" s="152" t="str">
+      <c r="S4" s="154"/>
+      <c r="T4" s="154"/>
+      <c r="U4" s="154"/>
+      <c r="V4" s="154"/>
+      <c r="W4" s="154"/>
+      <c r="X4" s="155"/>
+      <c r="Y4" s="153" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="Z4" s="153"/>
-      <c r="AA4" s="153"/>
-      <c r="AB4" s="153"/>
-      <c r="AC4" s="153"/>
-      <c r="AD4" s="153"/>
-      <c r="AE4" s="154"/>
-      <c r="AF4" s="152" t="str">
+      <c r="Z4" s="154"/>
+      <c r="AA4" s="154"/>
+      <c r="AB4" s="154"/>
+      <c r="AC4" s="154"/>
+      <c r="AD4" s="154"/>
+      <c r="AE4" s="155"/>
+      <c r="AF4" s="153" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="AG4" s="153"/>
-      <c r="AH4" s="153"/>
-      <c r="AI4" s="153"/>
-      <c r="AJ4" s="153"/>
-      <c r="AK4" s="153"/>
-      <c r="AL4" s="154"/>
-      <c r="AM4" s="152" t="str">
+      <c r="AG4" s="154"/>
+      <c r="AH4" s="154"/>
+      <c r="AI4" s="154"/>
+      <c r="AJ4" s="154"/>
+      <c r="AK4" s="154"/>
+      <c r="AL4" s="155"/>
+      <c r="AM4" s="153" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="AN4" s="153"/>
-      <c r="AO4" s="153"/>
-      <c r="AP4" s="153"/>
-      <c r="AQ4" s="153"/>
-      <c r="AR4" s="153"/>
-      <c r="AS4" s="154"/>
-      <c r="AT4" s="152" t="str">
+      <c r="AN4" s="154"/>
+      <c r="AO4" s="154"/>
+      <c r="AP4" s="154"/>
+      <c r="AQ4" s="154"/>
+      <c r="AR4" s="154"/>
+      <c r="AS4" s="155"/>
+      <c r="AT4" s="153" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="AU4" s="153"/>
-      <c r="AV4" s="153"/>
-      <c r="AW4" s="153"/>
-      <c r="AX4" s="153"/>
-      <c r="AY4" s="153"/>
-      <c r="AZ4" s="154"/>
-      <c r="BA4" s="152" t="str">
+      <c r="AU4" s="154"/>
+      <c r="AV4" s="154"/>
+      <c r="AW4" s="154"/>
+      <c r="AX4" s="154"/>
+      <c r="AY4" s="154"/>
+      <c r="AZ4" s="155"/>
+      <c r="BA4" s="153" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BB4" s="153"/>
-      <c r="BC4" s="153"/>
-      <c r="BD4" s="153"/>
-      <c r="BE4" s="153"/>
-      <c r="BF4" s="153"/>
-      <c r="BG4" s="154"/>
-      <c r="BH4" s="152" t="str">
+      <c r="BB4" s="154"/>
+      <c r="BC4" s="154"/>
+      <c r="BD4" s="154"/>
+      <c r="BE4" s="154"/>
+      <c r="BF4" s="154"/>
+      <c r="BG4" s="155"/>
+      <c r="BH4" s="153" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="BI4" s="153"/>
-      <c r="BJ4" s="153"/>
-      <c r="BK4" s="153"/>
-      <c r="BL4" s="153"/>
-      <c r="BM4" s="153"/>
-      <c r="BN4" s="154"/>
-      <c r="BO4" s="152" t="str">
+      <c r="BI4" s="154"/>
+      <c r="BJ4" s="154"/>
+      <c r="BK4" s="154"/>
+      <c r="BL4" s="154"/>
+      <c r="BM4" s="154"/>
+      <c r="BN4" s="155"/>
+      <c r="BO4" s="153" t="str">
         <f>"Week "&amp;(BO6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="BP4" s="153"/>
-      <c r="BQ4" s="153"/>
-      <c r="BR4" s="153"/>
-      <c r="BS4" s="153"/>
-      <c r="BT4" s="153"/>
-      <c r="BU4" s="154"/>
-      <c r="BV4" s="152" t="str">
+      <c r="BP4" s="154"/>
+      <c r="BQ4" s="154"/>
+      <c r="BR4" s="154"/>
+      <c r="BS4" s="154"/>
+      <c r="BT4" s="154"/>
+      <c r="BU4" s="155"/>
+      <c r="BV4" s="153" t="str">
         <f t="shared" ref="BV4" si="0">"Week "&amp;(BV6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="BW4" s="153"/>
-      <c r="BX4" s="153"/>
-      <c r="BY4" s="153"/>
-      <c r="BZ4" s="153"/>
-      <c r="CA4" s="153"/>
-      <c r="CB4" s="154"/>
-      <c r="CC4" s="152" t="str">
+      <c r="BW4" s="154"/>
+      <c r="BX4" s="154"/>
+      <c r="BY4" s="154"/>
+      <c r="BZ4" s="154"/>
+      <c r="CA4" s="154"/>
+      <c r="CB4" s="155"/>
+      <c r="CC4" s="153" t="str">
         <f t="shared" ref="CC4" si="1">"Week "&amp;(CC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="CD4" s="153"/>
-      <c r="CE4" s="153"/>
-      <c r="CF4" s="153"/>
-      <c r="CG4" s="153"/>
-      <c r="CH4" s="153"/>
-      <c r="CI4" s="154"/>
+      <c r="CD4" s="154"/>
+      <c r="CE4" s="154"/>
+      <c r="CF4" s="154"/>
+      <c r="CG4" s="154"/>
+      <c r="CH4" s="154"/>
+      <c r="CI4" s="155"/>
     </row>
     <row r="5" spans="1:87" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="90"/>
       <c r="B5" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="151"/>
-      <c r="D5" s="151"/>
-      <c r="E5" s="151"/>
+      <c r="C5" s="157"/>
+      <c r="D5" s="157"/>
+      <c r="E5" s="157"/>
       <c r="F5" s="93"/>
       <c r="G5" s="93"/>
       <c r="H5" s="93"/>
       <c r="I5" s="93"/>
       <c r="J5" s="46"/>
-      <c r="K5" s="156">
+      <c r="K5" s="150">
         <f>K6</f>
         <v>43871</v>
       </c>
-      <c r="L5" s="157"/>
-      <c r="M5" s="157"/>
-      <c r="N5" s="157"/>
-      <c r="O5" s="157"/>
-      <c r="P5" s="157"/>
-      <c r="Q5" s="158"/>
-      <c r="R5" s="156">
+      <c r="L5" s="151"/>
+      <c r="M5" s="151"/>
+      <c r="N5" s="151"/>
+      <c r="O5" s="151"/>
+      <c r="P5" s="151"/>
+      <c r="Q5" s="152"/>
+      <c r="R5" s="150">
         <f>R6</f>
         <v>43878</v>
       </c>
-      <c r="S5" s="157"/>
-      <c r="T5" s="157"/>
-      <c r="U5" s="157"/>
-      <c r="V5" s="157"/>
-      <c r="W5" s="157"/>
-      <c r="X5" s="158"/>
-      <c r="Y5" s="156">
+      <c r="S5" s="151"/>
+      <c r="T5" s="151"/>
+      <c r="U5" s="151"/>
+      <c r="V5" s="151"/>
+      <c r="W5" s="151"/>
+      <c r="X5" s="152"/>
+      <c r="Y5" s="150">
         <f>Y6</f>
         <v>43885</v>
       </c>
-      <c r="Z5" s="157"/>
-      <c r="AA5" s="157"/>
-      <c r="AB5" s="157"/>
-      <c r="AC5" s="157"/>
-      <c r="AD5" s="157"/>
-      <c r="AE5" s="158"/>
-      <c r="AF5" s="156">
+      <c r="Z5" s="151"/>
+      <c r="AA5" s="151"/>
+      <c r="AB5" s="151"/>
+      <c r="AC5" s="151"/>
+      <c r="AD5" s="151"/>
+      <c r="AE5" s="152"/>
+      <c r="AF5" s="150">
         <f>AF6</f>
         <v>43892</v>
       </c>
-      <c r="AG5" s="157"/>
-      <c r="AH5" s="157"/>
-      <c r="AI5" s="157"/>
-      <c r="AJ5" s="157"/>
-      <c r="AK5" s="157"/>
-      <c r="AL5" s="158"/>
-      <c r="AM5" s="156">
+      <c r="AG5" s="151"/>
+      <c r="AH5" s="151"/>
+      <c r="AI5" s="151"/>
+      <c r="AJ5" s="151"/>
+      <c r="AK5" s="151"/>
+      <c r="AL5" s="152"/>
+      <c r="AM5" s="150">
         <f>AM6</f>
         <v>43899</v>
       </c>
-      <c r="AN5" s="157"/>
-      <c r="AO5" s="157"/>
-      <c r="AP5" s="157"/>
-      <c r="AQ5" s="157"/>
-      <c r="AR5" s="157"/>
-      <c r="AS5" s="158"/>
-      <c r="AT5" s="156">
+      <c r="AN5" s="151"/>
+      <c r="AO5" s="151"/>
+      <c r="AP5" s="151"/>
+      <c r="AQ5" s="151"/>
+      <c r="AR5" s="151"/>
+      <c r="AS5" s="152"/>
+      <c r="AT5" s="150">
         <f>AT6</f>
         <v>43906</v>
       </c>
-      <c r="AU5" s="157"/>
-      <c r="AV5" s="157"/>
-      <c r="AW5" s="157"/>
-      <c r="AX5" s="157"/>
-      <c r="AY5" s="157"/>
-      <c r="AZ5" s="158"/>
-      <c r="BA5" s="156">
+      <c r="AU5" s="151"/>
+      <c r="AV5" s="151"/>
+      <c r="AW5" s="151"/>
+      <c r="AX5" s="151"/>
+      <c r="AY5" s="151"/>
+      <c r="AZ5" s="152"/>
+      <c r="BA5" s="150">
         <f>BA6</f>
         <v>43913</v>
       </c>
-      <c r="BB5" s="157"/>
-      <c r="BC5" s="157"/>
-      <c r="BD5" s="157"/>
-      <c r="BE5" s="157"/>
-      <c r="BF5" s="157"/>
-      <c r="BG5" s="158"/>
-      <c r="BH5" s="156">
+      <c r="BB5" s="151"/>
+      <c r="BC5" s="151"/>
+      <c r="BD5" s="151"/>
+      <c r="BE5" s="151"/>
+      <c r="BF5" s="151"/>
+      <c r="BG5" s="152"/>
+      <c r="BH5" s="150">
         <f>BH6</f>
         <v>43920</v>
       </c>
-      <c r="BI5" s="157"/>
-      <c r="BJ5" s="157"/>
-      <c r="BK5" s="157"/>
-      <c r="BL5" s="157"/>
-      <c r="BM5" s="157"/>
-      <c r="BN5" s="158"/>
-      <c r="BO5" s="156">
+      <c r="BI5" s="151"/>
+      <c r="BJ5" s="151"/>
+      <c r="BK5" s="151"/>
+      <c r="BL5" s="151"/>
+      <c r="BM5" s="151"/>
+      <c r="BN5" s="152"/>
+      <c r="BO5" s="150">
         <f>BO6</f>
         <v>43927</v>
       </c>
-      <c r="BP5" s="157"/>
-      <c r="BQ5" s="157"/>
-      <c r="BR5" s="157"/>
-      <c r="BS5" s="157"/>
-      <c r="BT5" s="157"/>
-      <c r="BU5" s="158"/>
-      <c r="BV5" s="156">
+      <c r="BP5" s="151"/>
+      <c r="BQ5" s="151"/>
+      <c r="BR5" s="151"/>
+      <c r="BS5" s="151"/>
+      <c r="BT5" s="151"/>
+      <c r="BU5" s="152"/>
+      <c r="BV5" s="150">
         <f t="shared" ref="BV5" si="2">BV6</f>
         <v>43934</v>
       </c>
-      <c r="BW5" s="157"/>
-      <c r="BX5" s="157"/>
-      <c r="BY5" s="157"/>
-      <c r="BZ5" s="157"/>
-      <c r="CA5" s="157"/>
-      <c r="CB5" s="158"/>
-      <c r="CC5" s="156">
+      <c r="BW5" s="151"/>
+      <c r="BX5" s="151"/>
+      <c r="BY5" s="151"/>
+      <c r="BZ5" s="151"/>
+      <c r="CA5" s="151"/>
+      <c r="CB5" s="152"/>
+      <c r="CC5" s="150">
         <f t="shared" ref="CC5" si="3">CC6</f>
         <v>43941</v>
       </c>
-      <c r="CD5" s="157"/>
-      <c r="CE5" s="157"/>
-      <c r="CF5" s="157"/>
-      <c r="CG5" s="157"/>
-      <c r="CH5" s="157"/>
-      <c r="CI5" s="158"/>
+      <c r="CD5" s="151"/>
+      <c r="CE5" s="151"/>
+      <c r="CF5" s="151"/>
+      <c r="CG5" s="151"/>
+      <c r="CH5" s="151"/>
+      <c r="CI5" s="152"/>
     </row>
     <row r="6" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A6" s="45"/>
@@ -4939,7 +4951,7 @@
       <c r="G8" s="73"/>
       <c r="H8" s="74"/>
       <c r="I8" s="75" t="str">
-        <f t="shared" ref="I8:I75" si="31">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I76" si="31">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="78"/>
@@ -6141,7 +6153,7 @@
         <v>5</v>
       </c>
       <c r="H22" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="60">
         <f t="shared" si="31"/>
@@ -6210,7 +6222,7 @@
         <v>162</v>
       </c>
       <c r="B23" s="106" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C23" s="57" t="s">
         <v>138</v>
@@ -6226,7 +6238,7 @@
         <v>5</v>
       </c>
       <c r="H23" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="60">
         <v>5</v>
@@ -6291,10 +6303,10 @@
     </row>
     <row r="24" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="56" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="106" t="s">
         <v>197</v>
-      </c>
-      <c r="B24" s="106" t="s">
-        <v>198</v>
       </c>
       <c r="C24" s="57" t="s">
         <v>138</v>
@@ -6310,7 +6322,7 @@
         <v>5</v>
       </c>
       <c r="H24" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="60">
         <v>5</v>
@@ -6375,10 +6387,10 @@
     </row>
     <row r="25" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="56" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" s="106" t="s">
         <v>199</v>
-      </c>
-      <c r="B25" s="106" t="s">
-        <v>200</v>
       </c>
       <c r="C25" s="57" t="s">
         <v>138</v>
@@ -6394,7 +6406,7 @@
         <v>5</v>
       </c>
       <c r="H25" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="60">
         <v>5</v>
@@ -6459,10 +6471,10 @@
     </row>
     <row r="26" spans="1:66" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" s="106" t="s">
         <v>201</v>
-      </c>
-      <c r="B26" s="106" t="s">
-        <v>202</v>
       </c>
       <c r="C26" s="57" t="s">
         <v>138</v>
@@ -6478,7 +6490,7 @@
         <v>5</v>
       </c>
       <c r="H26" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="60">
         <v>5</v>
@@ -6543,10 +6555,10 @@
     </row>
     <row r="27" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A27" s="56" t="s">
+        <v>202</v>
+      </c>
+      <c r="B27" s="106" t="s">
         <v>203</v>
-      </c>
-      <c r="B27" s="106" t="s">
-        <v>204</v>
       </c>
       <c r="C27" s="57" t="s">
         <v>138</v>
@@ -6562,7 +6574,7 @@
         <v>5</v>
       </c>
       <c r="H27" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="60">
         <v>5</v>
@@ -6627,10 +6639,10 @@
     </row>
     <row r="28" spans="1:66" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="56" t="s">
+        <v>204</v>
+      </c>
+      <c r="B28" s="106" t="s">
         <v>205</v>
-      </c>
-      <c r="B28" s="106" t="s">
-        <v>206</v>
       </c>
       <c r="C28" s="57" t="s">
         <v>138</v>
@@ -6646,7 +6658,7 @@
         <v>5</v>
       </c>
       <c r="H28" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="60">
         <v>5</v>
@@ -6731,7 +6743,7 @@
         <v>5</v>
       </c>
       <c r="H29" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="60">
         <f t="shared" si="31"/>
@@ -6893,10 +6905,10 @@
       </c>
       <c r="D31" s="107"/>
       <c r="E31" s="82">
-        <v>43906</v>
+        <v>43927</v>
       </c>
       <c r="F31" s="83">
-        <v>43910</v>
+        <v>43931</v>
       </c>
       <c r="G31" s="58">
         <v>5</v>
@@ -6978,11 +6990,11 @@
       </c>
       <c r="D32" s="141"/>
       <c r="E32" s="142">
-        <v>43913</v>
+        <v>43920</v>
       </c>
       <c r="F32" s="143">
         <f t="shared" si="33"/>
-        <v>43917</v>
+        <v>43924</v>
       </c>
       <c r="G32" s="144">
         <v>5</v>
@@ -7309,7 +7321,7 @@
         <v>3.3</v>
       </c>
       <c r="B36" s="106" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C36" s="57" t="s">
         <v>139</v>
@@ -7394,7 +7406,7 @@
         <v>3.4</v>
       </c>
       <c r="B37" s="106" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C37" s="57" t="s">
         <v>143</v>
@@ -7478,7 +7490,7 @@
         <v>3.5</v>
       </c>
       <c r="B38" s="106" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C38" s="57" t="s">
         <v>138</v>
@@ -7580,7 +7592,7 @@
         <v>5</v>
       </c>
       <c r="H39" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="60">
         <f t="shared" si="31"/>
@@ -7917,7 +7929,7 @@
         <v>3</v>
       </c>
       <c r="H43" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" s="60">
         <f t="shared" si="31"/>
@@ -8004,7 +8016,7 @@
         <v>3</v>
       </c>
       <c r="H44" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" s="60">
         <f t="shared" si="31"/>
@@ -8090,7 +8102,7 @@
         <v>1</v>
       </c>
       <c r="H45" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" s="60">
         <f t="shared" si="31"/>
@@ -8263,7 +8275,7 @@
         <v>1</v>
       </c>
       <c r="H47" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47" s="60">
         <f t="shared" si="31"/>
@@ -8338,13 +8350,13 @@
       <c r="D48" s="52"/>
       <c r="E48" s="84"/>
       <c r="F48" s="84" t="str">
-        <f t="shared" ref="F48:F50" si="34">IF(ISBLANK(E48)," - ",IF(G48=0,E48,E48+G48-1))</f>
+        <f t="shared" ref="F48:F51" si="34">IF(ISBLANK(E48)," - ",IF(G48=0,E48,E48+G48-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G48" s="53"/>
       <c r="H48" s="54"/>
       <c r="I48" s="55" t="str">
-        <f t="shared" ref="I48:I50" si="35">IF(OR(F48=0,E48=0)," - ",NETWORKDAYS(E48,F48))</f>
+        <f t="shared" ref="I48:I51" si="35">IF(OR(F48=0,E48=0)," - ",NETWORKDAYS(E48,F48))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J48" s="80"/>
@@ -8405,7 +8417,7 @@
       <c r="BM48" s="89"/>
       <c r="BN48" s="89"/>
     </row>
-    <row r="49" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:78" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A49" s="56" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
@@ -8492,24 +8504,24 @@
       <c r="BM49" s="87"/>
       <c r="BN49" s="87"/>
     </row>
-    <row r="50" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:78" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A50" s="56" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.2</v>
       </c>
       <c r="B50" s="106" t="s">
-        <v>171</v>
+        <v>207</v>
       </c>
       <c r="C50" s="57" t="s">
         <v>153</v>
       </c>
       <c r="D50" s="107"/>
       <c r="E50" s="82">
-        <v>43899</v>
+        <v>43934</v>
       </c>
       <c r="F50" s="83">
         <f t="shared" si="34"/>
-        <v>43901</v>
+        <v>43936</v>
       </c>
       <c r="G50" s="58">
         <v>3</v>
@@ -8578,32 +8590,35 @@
       <c r="BL50" s="87"/>
       <c r="BM50" s="87"/>
       <c r="BN50" s="87"/>
-    </row>
-    <row r="51" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A51" s="56">
-        <v>5.3</v>
-      </c>
+      <c r="BV50" s="160"/>
+      <c r="BW50" s="160"/>
+      <c r="BX50" s="160"/>
+    </row>
+    <row r="51" spans="1:78" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A51" s="56"/>
       <c r="B51" s="106" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
       <c r="C51" s="57" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D51" s="141"/>
-      <c r="E51" s="142">
-        <v>43880</v>
-      </c>
-      <c r="F51" s="143">
-        <v>43880</v>
-      </c>
-      <c r="G51" s="144">
-        <v>1</v>
-      </c>
-      <c r="H51" s="145">
-        <v>1</v>
-      </c>
-      <c r="I51" s="146">
-        <v>1</v>
+      <c r="E51" s="82">
+        <v>43935</v>
+      </c>
+      <c r="F51" s="83">
+        <f t="shared" si="34"/>
+        <v>43937</v>
+      </c>
+      <c r="G51" s="58">
+        <v>3</v>
+      </c>
+      <c r="H51" s="59">
+        <v>0</v>
+      </c>
+      <c r="I51" s="60">
+        <f t="shared" si="35"/>
+        <v>3</v>
       </c>
       <c r="J51" s="147"/>
       <c r="K51" s="87"/>
@@ -8662,23 +8677,26 @@
       <c r="BL51" s="87"/>
       <c r="BM51" s="87"/>
       <c r="BN51" s="87"/>
-    </row>
-    <row r="52" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="BV51" s="160"/>
+      <c r="BW51" s="160"/>
+      <c r="BX51" s="160"/>
+    </row>
+    <row r="52" spans="1:78" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A52" s="56">
-        <v>5.4</v>
+        <v>5.3</v>
       </c>
       <c r="B52" s="106" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C52" s="57" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D52" s="141"/>
       <c r="E52" s="142">
-        <v>43885</v>
+        <v>43880</v>
       </c>
       <c r="F52" s="143">
-        <v>43885</v>
+        <v>43880</v>
       </c>
       <c r="G52" s="144">
         <v>1</v>
@@ -8747,28 +8765,28 @@
       <c r="BM52" s="87"/>
       <c r="BN52" s="87"/>
     </row>
-    <row r="53" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:78" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A53" s="56">
-        <v>5.5</v>
+        <v>5.4</v>
       </c>
       <c r="B53" s="106" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C53" s="57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D53" s="141"/>
       <c r="E53" s="142">
-        <v>43899</v>
+        <v>43885</v>
       </c>
       <c r="F53" s="143">
-        <v>43899</v>
+        <v>43885</v>
       </c>
       <c r="G53" s="144">
         <v>1</v>
       </c>
       <c r="H53" s="145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="146">
         <v>1</v>
@@ -8831,15 +8849,15 @@
       <c r="BM53" s="87"/>
       <c r="BN53" s="87"/>
     </row>
-    <row r="54" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:78" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A54" s="56">
-        <v>5.6</v>
+        <v>5.5</v>
       </c>
       <c r="B54" s="106" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="C54" s="57" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D54" s="141"/>
       <c r="E54" s="142">
@@ -8852,7 +8870,7 @@
         <v>1</v>
       </c>
       <c r="H54" s="145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" s="146">
         <v>1</v>
@@ -8915,28 +8933,28 @@
       <c r="BM54" s="87"/>
       <c r="BN54" s="87"/>
     </row>
-    <row r="55" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:78" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A55" s="56">
-        <v>5.7</v>
+        <v>5.6</v>
       </c>
       <c r="B55" s="106" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="C55" s="57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D55" s="141"/>
       <c r="E55" s="142">
-        <v>43906</v>
+        <v>43899</v>
       </c>
       <c r="F55" s="143">
-        <v>43906</v>
+        <v>43899</v>
       </c>
       <c r="G55" s="144">
         <v>1</v>
       </c>
       <c r="H55" s="145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" s="146">
         <v>1</v>
@@ -8999,15 +9017,15 @@
       <c r="BM55" s="87"/>
       <c r="BN55" s="87"/>
     </row>
-    <row r="56" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:78" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A56" s="56">
-        <v>5.8</v>
+        <v>5.7</v>
       </c>
       <c r="B56" s="106" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C56" s="57" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D56" s="141"/>
       <c r="E56" s="142">
@@ -9020,7 +9038,7 @@
         <v>1</v>
       </c>
       <c r="H56" s="145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" s="146">
         <v>1</v>
@@ -9083,22 +9101,22 @@
       <c r="BM56" s="87"/>
       <c r="BN56" s="87"/>
     </row>
-    <row r="57" spans="1:71" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:78" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="56">
-        <v>5.9</v>
+        <v>5.8</v>
       </c>
       <c r="B57" s="106" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C57" s="57" t="s">
         <v>138</v>
       </c>
       <c r="D57" s="141"/>
       <c r="E57" s="142">
-        <v>43913</v>
+        <v>43934</v>
       </c>
       <c r="F57" s="143">
-        <v>43913</v>
+        <v>43934</v>
       </c>
       <c r="G57" s="144">
         <v>1</v>
@@ -9167,201 +9185,196 @@
       <c r="BM57" s="87"/>
       <c r="BN57" s="87"/>
     </row>
-    <row r="58" spans="1:71" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A58" s="49" t="str">
+    <row r="58" spans="1:78" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="56">
+        <v>5.9</v>
+      </c>
+      <c r="B58" s="106" t="s">
+        <v>191</v>
+      </c>
+      <c r="C58" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="141"/>
+      <c r="E58" s="142">
+        <v>43927</v>
+      </c>
+      <c r="F58" s="143">
+        <v>43927</v>
+      </c>
+      <c r="G58" s="144">
+        <v>1</v>
+      </c>
+      <c r="H58" s="145">
+        <v>0</v>
+      </c>
+      <c r="I58" s="146">
+        <v>1</v>
+      </c>
+      <c r="J58" s="147"/>
+      <c r="K58" s="87"/>
+      <c r="L58" s="87"/>
+      <c r="M58" s="87"/>
+      <c r="N58" s="87"/>
+      <c r="O58" s="87"/>
+      <c r="P58" s="87"/>
+      <c r="Q58" s="87"/>
+      <c r="R58" s="87"/>
+      <c r="S58" s="87"/>
+      <c r="T58" s="87"/>
+      <c r="U58" s="87"/>
+      <c r="V58" s="87"/>
+      <c r="W58" s="87"/>
+      <c r="X58" s="87"/>
+      <c r="Y58" s="87"/>
+      <c r="Z58" s="87"/>
+      <c r="AA58" s="87"/>
+      <c r="AB58" s="87"/>
+      <c r="AC58" s="87"/>
+      <c r="AD58" s="87"/>
+      <c r="AE58" s="87"/>
+      <c r="AF58" s="87"/>
+      <c r="AG58" s="87"/>
+      <c r="AH58" s="87"/>
+      <c r="AI58" s="87"/>
+      <c r="AJ58" s="87"/>
+      <c r="AK58" s="87"/>
+      <c r="AL58" s="87"/>
+      <c r="AM58" s="87"/>
+      <c r="AN58" s="87"/>
+      <c r="AO58" s="87"/>
+      <c r="AP58" s="87"/>
+      <c r="AQ58" s="87"/>
+      <c r="AR58" s="87"/>
+      <c r="AS58" s="87"/>
+      <c r="AT58" s="87"/>
+      <c r="AU58" s="87"/>
+      <c r="AV58" s="87"/>
+      <c r="AW58" s="87"/>
+      <c r="AX58" s="87"/>
+      <c r="AY58" s="87"/>
+      <c r="AZ58" s="87"/>
+      <c r="BA58" s="87"/>
+      <c r="BB58" s="87"/>
+      <c r="BC58" s="87"/>
+      <c r="BD58" s="87"/>
+      <c r="BE58" s="87"/>
+      <c r="BF58" s="87"/>
+      <c r="BG58" s="87"/>
+      <c r="BH58" s="87"/>
+      <c r="BI58" s="87"/>
+      <c r="BJ58" s="87"/>
+      <c r="BK58" s="87"/>
+      <c r="BL58" s="87"/>
+      <c r="BM58" s="87"/>
+      <c r="BN58" s="87"/>
+    </row>
+    <row r="59" spans="1:78" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="49" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>6</v>
       </c>
-      <c r="B58" s="50" t="s">
+      <c r="B59" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="D59" s="52"/>
+      <c r="E59" s="84"/>
+      <c r="F59" s="84" t="str">
+        <f t="shared" ref="F59" si="36">IF(ISBLANK(E59)," - ",IF(G59=0,E59,E59+G59-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G59" s="53"/>
+      <c r="H59" s="54"/>
+      <c r="I59" s="55" t="str">
+        <f t="shared" ref="I59:I60" si="37">IF(OR(F59=0,E59=0)," - ",NETWORKDAYS(E59,F59))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J59" s="80"/>
+      <c r="K59" s="89"/>
+      <c r="L59" s="89"/>
+      <c r="M59" s="89"/>
+      <c r="N59" s="89"/>
+      <c r="O59" s="89"/>
+      <c r="P59" s="89"/>
+      <c r="Q59" s="89"/>
+      <c r="R59" s="89"/>
+      <c r="S59" s="89"/>
+      <c r="T59" s="89"/>
+      <c r="U59" s="89"/>
+      <c r="V59" s="89"/>
+      <c r="W59" s="89"/>
+      <c r="X59" s="89"/>
+      <c r="Y59" s="89"/>
+      <c r="Z59" s="89"/>
+      <c r="AA59" s="89"/>
+      <c r="AB59" s="89"/>
+      <c r="AC59" s="89"/>
+      <c r="AD59" s="89"/>
+      <c r="AE59" s="89"/>
+      <c r="AF59" s="89"/>
+      <c r="AG59" s="89"/>
+      <c r="AH59" s="89"/>
+      <c r="AI59" s="89"/>
+      <c r="AJ59" s="89"/>
+      <c r="AK59" s="89"/>
+      <c r="AL59" s="89"/>
+      <c r="AM59" s="89"/>
+      <c r="AN59" s="89"/>
+      <c r="AO59" s="89"/>
+      <c r="AP59" s="89"/>
+      <c r="AQ59" s="89"/>
+      <c r="AR59" s="89"/>
+      <c r="AS59" s="89"/>
+      <c r="AT59" s="89"/>
+      <c r="AU59" s="89"/>
+      <c r="AV59" s="89"/>
+      <c r="AW59" s="89"/>
+      <c r="AX59" s="89"/>
+      <c r="AY59" s="89"/>
+      <c r="AZ59" s="89"/>
+      <c r="BA59" s="89"/>
+      <c r="BB59" s="89"/>
+      <c r="BC59" s="89"/>
+      <c r="BD59" s="89"/>
+      <c r="BE59" s="89"/>
+      <c r="BF59" s="89"/>
+      <c r="BG59" s="89"/>
+      <c r="BH59" s="89"/>
+      <c r="BI59" s="89"/>
+      <c r="BJ59" s="89"/>
+      <c r="BK59" s="89"/>
+      <c r="BL59" s="89"/>
+      <c r="BM59" s="89"/>
+      <c r="BN59" s="89"/>
+    </row>
+    <row r="60" spans="1:78" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="56">
+        <v>6.1</v>
+      </c>
+      <c r="B60" s="106" t="s">
         <v>193</v>
       </c>
-      <c r="D58" s="52"/>
-      <c r="E58" s="84"/>
-      <c r="F58" s="84" t="str">
-        <f t="shared" ref="F58" si="36">IF(ISBLANK(E58)," - ",IF(G58=0,E58,E58+G58-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G58" s="53"/>
-      <c r="H58" s="54"/>
-      <c r="I58" s="55" t="str">
-        <f t="shared" ref="I58:I59" si="37">IF(OR(F58=0,E58=0)," - ",NETWORKDAYS(E58,F58))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J58" s="80"/>
-      <c r="K58" s="89"/>
-      <c r="L58" s="89"/>
-      <c r="M58" s="89"/>
-      <c r="N58" s="89"/>
-      <c r="O58" s="89"/>
-      <c r="P58" s="89"/>
-      <c r="Q58" s="89"/>
-      <c r="R58" s="89"/>
-      <c r="S58" s="89"/>
-      <c r="T58" s="89"/>
-      <c r="U58" s="89"/>
-      <c r="V58" s="89"/>
-      <c r="W58" s="89"/>
-      <c r="X58" s="89"/>
-      <c r="Y58" s="89"/>
-      <c r="Z58" s="89"/>
-      <c r="AA58" s="89"/>
-      <c r="AB58" s="89"/>
-      <c r="AC58" s="89"/>
-      <c r="AD58" s="89"/>
-      <c r="AE58" s="89"/>
-      <c r="AF58" s="89"/>
-      <c r="AG58" s="89"/>
-      <c r="AH58" s="89"/>
-      <c r="AI58" s="89"/>
-      <c r="AJ58" s="89"/>
-      <c r="AK58" s="89"/>
-      <c r="AL58" s="89"/>
-      <c r="AM58" s="89"/>
-      <c r="AN58" s="89"/>
-      <c r="AO58" s="89"/>
-      <c r="AP58" s="89"/>
-      <c r="AQ58" s="89"/>
-      <c r="AR58" s="89"/>
-      <c r="AS58" s="89"/>
-      <c r="AT58" s="89"/>
-      <c r="AU58" s="89"/>
-      <c r="AV58" s="89"/>
-      <c r="AW58" s="89"/>
-      <c r="AX58" s="89"/>
-      <c r="AY58" s="89"/>
-      <c r="AZ58" s="89"/>
-      <c r="BA58" s="89"/>
-      <c r="BB58" s="89"/>
-      <c r="BC58" s="89"/>
-      <c r="BD58" s="89"/>
-      <c r="BE58" s="89"/>
-      <c r="BF58" s="89"/>
-      <c r="BG58" s="89"/>
-      <c r="BH58" s="89"/>
-      <c r="BI58" s="89"/>
-      <c r="BJ58" s="89"/>
-      <c r="BK58" s="89"/>
-      <c r="BL58" s="89"/>
-      <c r="BM58" s="89"/>
-      <c r="BN58" s="89"/>
-    </row>
-    <row r="59" spans="1:71" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A59" s="56">
-        <v>6.1</v>
-      </c>
-      <c r="B59" s="106" t="s">
-        <v>194</v>
-      </c>
-      <c r="C59" s="57" t="s">
+      <c r="C60" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="D59" s="107"/>
-      <c r="E59" s="82">
+      <c r="D60" s="107"/>
+      <c r="E60" s="82">
         <v>43913</v>
       </c>
-      <c r="F59" s="83">
+      <c r="F60" s="83">
         <v>43917</v>
       </c>
-      <c r="G59" s="58">
+      <c r="G60" s="58">
         <v>2</v>
       </c>
-      <c r="H59" s="59">
+      <c r="H60" s="59">
         <v>0</v>
       </c>
-      <c r="I59" s="60">
+      <c r="I60" s="60">
         <f t="shared" si="37"/>
         <v>5</v>
       </c>
-      <c r="J59" s="79"/>
-      <c r="K59" s="87"/>
-      <c r="L59" s="87"/>
-      <c r="M59" s="87"/>
-      <c r="N59" s="87"/>
-      <c r="O59" s="87"/>
-      <c r="P59" s="87"/>
-      <c r="Q59" s="87"/>
-      <c r="R59" s="87"/>
-      <c r="S59" s="87"/>
-      <c r="T59" s="87"/>
-      <c r="U59" s="87"/>
-      <c r="V59" s="87"/>
-      <c r="W59" s="87"/>
-      <c r="X59" s="87"/>
-      <c r="Y59" s="87"/>
-      <c r="Z59" s="87"/>
-      <c r="AA59" s="87"/>
-      <c r="AB59" s="87"/>
-      <c r="AC59" s="87"/>
-      <c r="AD59" s="87"/>
-      <c r="AE59" s="87"/>
-      <c r="AF59" s="87"/>
-      <c r="AG59" s="87"/>
-      <c r="AH59" s="87"/>
-      <c r="AI59" s="87"/>
-      <c r="AJ59" s="87"/>
-      <c r="AK59" s="87"/>
-      <c r="AL59" s="87"/>
-      <c r="AM59" s="87"/>
-      <c r="AN59" s="87"/>
-      <c r="AO59" s="87"/>
-      <c r="AP59" s="87"/>
-      <c r="AQ59" s="87"/>
-      <c r="AR59" s="87"/>
-      <c r="AS59" s="87"/>
-      <c r="AT59" s="87"/>
-      <c r="AU59" s="87"/>
-      <c r="AV59" s="87"/>
-      <c r="AW59" s="87"/>
-      <c r="AX59" s="87"/>
-      <c r="AY59" s="87"/>
-      <c r="AZ59" s="87"/>
-      <c r="BA59" s="87"/>
-      <c r="BB59" s="87"/>
-      <c r="BC59" s="87"/>
-      <c r="BD59" s="87"/>
-      <c r="BE59" s="87"/>
-      <c r="BF59" s="87"/>
-      <c r="BG59" s="87"/>
-      <c r="BH59" s="87"/>
-      <c r="BI59" s="87"/>
-      <c r="BJ59" s="87"/>
-      <c r="BK59" s="87"/>
-      <c r="BL59" s="87"/>
-      <c r="BM59" s="87"/>
-      <c r="BN59" s="87"/>
-      <c r="BO59" s="149"/>
-      <c r="BP59" s="149"/>
-      <c r="BQ59" s="149"/>
-      <c r="BR59" s="149"/>
-      <c r="BS59" s="149"/>
-    </row>
-    <row r="60" spans="1:71" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A60" s="56">
-        <v>6.2</v>
-      </c>
-      <c r="B60" s="106" t="s">
-        <v>195</v>
-      </c>
-      <c r="C60" s="57" t="s">
-        <v>163</v>
-      </c>
-      <c r="D60" s="141"/>
-      <c r="E60" s="142">
-        <v>43920</v>
-      </c>
-      <c r="F60" s="143">
-        <v>43924</v>
-      </c>
-      <c r="G60" s="144">
-        <v>2</v>
-      </c>
-      <c r="H60" s="145">
-        <v>0</v>
-      </c>
-      <c r="I60" s="146">
-        <v>5</v>
-      </c>
-      <c r="J60" s="147"/>
+      <c r="J60" s="79"/>
       <c r="K60" s="87"/>
       <c r="L60" s="87"/>
       <c r="M60" s="87"/>
@@ -9424,190 +9437,189 @@
       <c r="BR60" s="149"/>
       <c r="BS60" s="149"/>
     </row>
-    <row r="61" spans="1:71" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A61" s="49" t="str">
+    <row r="61" spans="1:78" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="56">
+        <v>6.2</v>
+      </c>
+      <c r="B61" s="106" t="s">
+        <v>194</v>
+      </c>
+      <c r="C61" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="D61" s="141"/>
+      <c r="E61" s="142">
+        <v>43920</v>
+      </c>
+      <c r="F61" s="143">
+        <v>43924</v>
+      </c>
+      <c r="G61" s="144">
+        <v>2</v>
+      </c>
+      <c r="H61" s="145">
+        <v>0</v>
+      </c>
+      <c r="I61" s="146">
+        <v>5</v>
+      </c>
+      <c r="J61" s="147"/>
+      <c r="K61" s="87"/>
+      <c r="L61" s="87"/>
+      <c r="M61" s="87"/>
+      <c r="N61" s="87"/>
+      <c r="O61" s="87"/>
+      <c r="P61" s="87"/>
+      <c r="Q61" s="87"/>
+      <c r="R61" s="87"/>
+      <c r="S61" s="87"/>
+      <c r="T61" s="87"/>
+      <c r="U61" s="87"/>
+      <c r="V61" s="87"/>
+      <c r="W61" s="87"/>
+      <c r="X61" s="87"/>
+      <c r="Y61" s="87"/>
+      <c r="Z61" s="87"/>
+      <c r="AA61" s="87"/>
+      <c r="AB61" s="87"/>
+      <c r="AC61" s="87"/>
+      <c r="AD61" s="87"/>
+      <c r="AE61" s="87"/>
+      <c r="AF61" s="87"/>
+      <c r="AG61" s="87"/>
+      <c r="AH61" s="87"/>
+      <c r="AI61" s="87"/>
+      <c r="AJ61" s="87"/>
+      <c r="AK61" s="87"/>
+      <c r="AL61" s="87"/>
+      <c r="AM61" s="87"/>
+      <c r="AN61" s="87"/>
+      <c r="AO61" s="87"/>
+      <c r="AP61" s="87"/>
+      <c r="AQ61" s="87"/>
+      <c r="AR61" s="87"/>
+      <c r="AS61" s="87"/>
+      <c r="AT61" s="87"/>
+      <c r="AU61" s="87"/>
+      <c r="AV61" s="87"/>
+      <c r="AW61" s="87"/>
+      <c r="AX61" s="87"/>
+      <c r="AY61" s="87"/>
+      <c r="AZ61" s="87"/>
+      <c r="BA61" s="87"/>
+      <c r="BB61" s="87"/>
+      <c r="BC61" s="87"/>
+      <c r="BD61" s="87"/>
+      <c r="BE61" s="87"/>
+      <c r="BF61" s="87"/>
+      <c r="BG61" s="87"/>
+      <c r="BH61" s="87"/>
+      <c r="BI61" s="87"/>
+      <c r="BJ61" s="87"/>
+      <c r="BK61" s="87"/>
+      <c r="BL61" s="87"/>
+      <c r="BM61" s="87"/>
+      <c r="BN61" s="87"/>
+      <c r="BO61" s="149"/>
+      <c r="BP61" s="149"/>
+      <c r="BQ61" s="149"/>
+      <c r="BR61" s="149"/>
+      <c r="BS61" s="149"/>
+    </row>
+    <row r="62" spans="1:78" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="49" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>7</v>
       </c>
-      <c r="B61" s="50" t="s">
+      <c r="B62" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="D62" s="52"/>
+      <c r="E62" s="84"/>
+      <c r="F62" s="84" t="str">
+        <f t="shared" ref="F62" si="38">IF(ISBLANK(E62)," - ",IF(G62=0,E62,E62+G62-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G62" s="53"/>
+      <c r="H62" s="54"/>
+      <c r="I62" s="55" t="str">
+        <f t="shared" ref="I62:I68" si="39">IF(OR(F62=0,E62=0)," - ",NETWORKDAYS(E62,F62))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J62" s="80"/>
+      <c r="K62" s="89"/>
+      <c r="L62" s="89"/>
+      <c r="M62" s="89"/>
+      <c r="N62" s="89"/>
+      <c r="O62" s="89"/>
+      <c r="P62" s="89"/>
+      <c r="Q62" s="89"/>
+      <c r="R62" s="89"/>
+      <c r="S62" s="89"/>
+      <c r="T62" s="89"/>
+      <c r="U62" s="89"/>
+      <c r="V62" s="89"/>
+      <c r="W62" s="89"/>
+      <c r="X62" s="89"/>
+      <c r="Y62" s="89"/>
+      <c r="Z62" s="89"/>
+      <c r="AA62" s="89"/>
+      <c r="AB62" s="89"/>
+      <c r="AC62" s="89"/>
+      <c r="AD62" s="89"/>
+      <c r="AE62" s="89"/>
+      <c r="AF62" s="89"/>
+      <c r="AG62" s="89"/>
+      <c r="AH62" s="89"/>
+      <c r="AI62" s="89"/>
+      <c r="AJ62" s="89"/>
+      <c r="AK62" s="89"/>
+      <c r="AL62" s="89"/>
+      <c r="AM62" s="89"/>
+      <c r="AN62" s="89"/>
+      <c r="AO62" s="89"/>
+      <c r="AP62" s="89"/>
+      <c r="AQ62" s="89"/>
+      <c r="AR62" s="89"/>
+      <c r="AS62" s="89"/>
+      <c r="AT62" s="89"/>
+      <c r="AU62" s="89"/>
+      <c r="AV62" s="89"/>
+      <c r="AW62" s="89"/>
+      <c r="AX62" s="89"/>
+      <c r="AY62" s="89"/>
+      <c r="AZ62" s="89"/>
+      <c r="BA62" s="89"/>
+      <c r="BB62" s="89"/>
+      <c r="BC62" s="89"/>
+      <c r="BD62" s="89"/>
+      <c r="BE62" s="89"/>
+      <c r="BF62" s="89"/>
+      <c r="BG62" s="89"/>
+      <c r="BH62" s="89"/>
+      <c r="BI62" s="89"/>
+      <c r="BJ62" s="89"/>
+      <c r="BK62" s="89"/>
+      <c r="BL62" s="89"/>
+      <c r="BM62" s="89"/>
+      <c r="BN62" s="89"/>
+    </row>
+    <row r="63" spans="1:78" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A63" s="56">
+        <v>7.1</v>
+      </c>
+      <c r="B63" s="106" t="s">
         <v>172</v>
-      </c>
-      <c r="D61" s="52"/>
-      <c r="E61" s="84"/>
-      <c r="F61" s="84" t="str">
-        <f t="shared" ref="F61" si="38">IF(ISBLANK(E61)," - ",IF(G61=0,E61,E61+G61-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G61" s="53"/>
-      <c r="H61" s="54"/>
-      <c r="I61" s="55" t="str">
-        <f t="shared" ref="I61:I67" si="39">IF(OR(F61=0,E61=0)," - ",NETWORKDAYS(E61,F61))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J61" s="80"/>
-      <c r="K61" s="89"/>
-      <c r="L61" s="89"/>
-      <c r="M61" s="89"/>
-      <c r="N61" s="89"/>
-      <c r="O61" s="89"/>
-      <c r="P61" s="89"/>
-      <c r="Q61" s="89"/>
-      <c r="R61" s="89"/>
-      <c r="S61" s="89"/>
-      <c r="T61" s="89"/>
-      <c r="U61" s="89"/>
-      <c r="V61" s="89"/>
-      <c r="W61" s="89"/>
-      <c r="X61" s="89"/>
-      <c r="Y61" s="89"/>
-      <c r="Z61" s="89"/>
-      <c r="AA61" s="89"/>
-      <c r="AB61" s="89"/>
-      <c r="AC61" s="89"/>
-      <c r="AD61" s="89"/>
-      <c r="AE61" s="89"/>
-      <c r="AF61" s="89"/>
-      <c r="AG61" s="89"/>
-      <c r="AH61" s="89"/>
-      <c r="AI61" s="89"/>
-      <c r="AJ61" s="89"/>
-      <c r="AK61" s="89"/>
-      <c r="AL61" s="89"/>
-      <c r="AM61" s="89"/>
-      <c r="AN61" s="89"/>
-      <c r="AO61" s="89"/>
-      <c r="AP61" s="89"/>
-      <c r="AQ61" s="89"/>
-      <c r="AR61" s="89"/>
-      <c r="AS61" s="89"/>
-      <c r="AT61" s="89"/>
-      <c r="AU61" s="89"/>
-      <c r="AV61" s="89"/>
-      <c r="AW61" s="89"/>
-      <c r="AX61" s="89"/>
-      <c r="AY61" s="89"/>
-      <c r="AZ61" s="89"/>
-      <c r="BA61" s="89"/>
-      <c r="BB61" s="89"/>
-      <c r="BC61" s="89"/>
-      <c r="BD61" s="89"/>
-      <c r="BE61" s="89"/>
-      <c r="BF61" s="89"/>
-      <c r="BG61" s="89"/>
-      <c r="BH61" s="89"/>
-      <c r="BI61" s="89"/>
-      <c r="BJ61" s="89"/>
-      <c r="BK61" s="89"/>
-      <c r="BL61" s="89"/>
-      <c r="BM61" s="89"/>
-      <c r="BN61" s="89"/>
-    </row>
-    <row r="62" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A62" s="56">
-        <v>7.1</v>
-      </c>
-      <c r="B62" s="106" t="s">
-        <v>173</v>
-      </c>
-      <c r="C62" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="D62" s="107"/>
-      <c r="E62" s="82">
-        <v>43927</v>
-      </c>
-      <c r="F62" s="83">
-        <v>43931</v>
-      </c>
-      <c r="G62" s="58">
-        <v>2</v>
-      </c>
-      <c r="H62" s="59">
-        <v>0</v>
-      </c>
-      <c r="I62" s="60">
-        <f t="shared" si="39"/>
-        <v>5</v>
-      </c>
-      <c r="J62" s="79"/>
-      <c r="K62" s="87"/>
-      <c r="L62" s="87"/>
-      <c r="M62" s="87"/>
-      <c r="N62" s="87"/>
-      <c r="O62" s="87"/>
-      <c r="P62" s="87"/>
-      <c r="Q62" s="87"/>
-      <c r="R62" s="87"/>
-      <c r="S62" s="87"/>
-      <c r="T62" s="87"/>
-      <c r="U62" s="87"/>
-      <c r="V62" s="87"/>
-      <c r="W62" s="87"/>
-      <c r="X62" s="87"/>
-      <c r="Y62" s="87"/>
-      <c r="Z62" s="87"/>
-      <c r="AA62" s="87"/>
-      <c r="AB62" s="87"/>
-      <c r="AC62" s="87"/>
-      <c r="AD62" s="87"/>
-      <c r="AE62" s="87"/>
-      <c r="AF62" s="87"/>
-      <c r="AG62" s="87"/>
-      <c r="AH62" s="87"/>
-      <c r="AI62" s="87"/>
-      <c r="AJ62" s="87"/>
-      <c r="AK62" s="87"/>
-      <c r="AL62" s="87"/>
-      <c r="AM62" s="87"/>
-      <c r="AN62" s="87"/>
-      <c r="AO62" s="87"/>
-      <c r="AP62" s="87"/>
-      <c r="AQ62" s="87"/>
-      <c r="AR62" s="87"/>
-      <c r="AS62" s="87"/>
-      <c r="AT62" s="87"/>
-      <c r="AU62" s="87"/>
-      <c r="AV62" s="87"/>
-      <c r="AW62" s="87"/>
-      <c r="AX62" s="87"/>
-      <c r="AY62" s="87"/>
-      <c r="AZ62" s="87"/>
-      <c r="BA62" s="87"/>
-      <c r="BB62" s="87"/>
-      <c r="BC62" s="87"/>
-      <c r="BD62" s="87"/>
-      <c r="BE62" s="87"/>
-      <c r="BF62" s="87"/>
-      <c r="BG62" s="87"/>
-      <c r="BH62" s="87"/>
-      <c r="BI62" s="87"/>
-      <c r="BJ62" s="87"/>
-      <c r="BK62" s="87"/>
-      <c r="BL62" s="87"/>
-      <c r="BM62" s="87"/>
-      <c r="BN62" s="87"/>
-      <c r="BO62" s="148"/>
-      <c r="BP62" s="148"/>
-      <c r="BQ62" s="148"/>
-      <c r="BR62" s="148"/>
-      <c r="BS62" s="148"/>
-    </row>
-    <row r="63" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A63" s="56">
-        <v>7.2</v>
-      </c>
-      <c r="B63" s="106" t="s">
-        <v>174</v>
       </c>
       <c r="C63" s="57" t="s">
         <v>139</v>
       </c>
       <c r="D63" s="107"/>
       <c r="E63" s="82">
-        <v>43927</v>
+        <v>43934</v>
       </c>
       <c r="F63" s="83">
-        <v>43931</v>
+        <v>43938</v>
       </c>
       <c r="G63" s="58">
         <v>2</v>
@@ -9676,28 +9688,32 @@
       <c r="BL63" s="87"/>
       <c r="BM63" s="87"/>
       <c r="BN63" s="87"/>
-      <c r="BO63" s="148"/>
-      <c r="BP63" s="148"/>
-      <c r="BQ63" s="148"/>
-      <c r="BR63" s="148"/>
-      <c r="BS63" s="148"/>
-    </row>
-    <row r="64" spans="1:71" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="BO63" s="149"/>
+      <c r="BP63" s="149"/>
+      <c r="BQ63" s="149"/>
+      <c r="BR63" s="149"/>
+      <c r="BS63" s="149"/>
+      <c r="BW63" s="160"/>
+      <c r="BX63" s="160"/>
+      <c r="BY63" s="160"/>
+      <c r="BZ63" s="160"/>
+    </row>
+    <row r="64" spans="1:78" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A64" s="56">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="B64" s="106" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C64" s="57" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D64" s="107"/>
       <c r="E64" s="82">
-        <v>43927</v>
+        <v>43935</v>
       </c>
       <c r="F64" s="83">
-        <v>43931</v>
+        <v>43939</v>
       </c>
       <c r="G64" s="58">
         <v>2</v>
@@ -9707,7 +9723,7 @@
       </c>
       <c r="I64" s="60">
         <f t="shared" si="39"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J64" s="79"/>
       <c r="K64" s="87"/>
@@ -9766,28 +9782,32 @@
       <c r="BL64" s="87"/>
       <c r="BM64" s="87"/>
       <c r="BN64" s="87"/>
-      <c r="BO64" s="148"/>
-      <c r="BP64" s="148"/>
-      <c r="BQ64" s="148"/>
-      <c r="BR64" s="148"/>
-      <c r="BS64" s="148"/>
+      <c r="BO64" s="149"/>
+      <c r="BP64" s="149"/>
+      <c r="BQ64" s="149"/>
+      <c r="BR64" s="149"/>
+      <c r="BS64" s="149"/>
+      <c r="BW64" s="160"/>
+      <c r="BX64" s="160"/>
+      <c r="BY64" s="160"/>
+      <c r="BZ64" s="160"/>
     </row>
     <row r="65" spans="1:83" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A65" s="56">
-        <v>7.4</v>
+        <v>7.3</v>
       </c>
       <c r="B65" s="106" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C65" s="57" t="s">
         <v>138</v>
       </c>
       <c r="D65" s="107"/>
       <c r="E65" s="82">
-        <v>43927</v>
+        <v>43936</v>
       </c>
       <c r="F65" s="83">
-        <v>43931</v>
+        <v>43940</v>
       </c>
       <c r="G65" s="58">
         <v>2</v>
@@ -9797,7 +9817,7 @@
       </c>
       <c r="I65" s="60">
         <f t="shared" si="39"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J65" s="79"/>
       <c r="K65" s="87"/>
@@ -9856,28 +9876,32 @@
       <c r="BL65" s="87"/>
       <c r="BM65" s="87"/>
       <c r="BN65" s="87"/>
-      <c r="BO65" s="148"/>
-      <c r="BP65" s="148"/>
-      <c r="BQ65" s="148"/>
-      <c r="BR65" s="148"/>
-      <c r="BS65" s="148"/>
+      <c r="BO65" s="149"/>
+      <c r="BP65" s="149"/>
+      <c r="BQ65" s="149"/>
+      <c r="BR65" s="149"/>
+      <c r="BS65" s="149"/>
+      <c r="BW65" s="160"/>
+      <c r="BX65" s="160"/>
+      <c r="BY65" s="160"/>
+      <c r="BZ65" s="160"/>
     </row>
     <row r="66" spans="1:83" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A66" s="56">
-        <v>7.5</v>
+        <v>7.4</v>
       </c>
       <c r="B66" s="106" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C66" s="57" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D66" s="107"/>
       <c r="E66" s="82">
-        <v>43927</v>
+        <v>43937</v>
       </c>
       <c r="F66" s="83">
-        <v>43931</v>
+        <v>43941</v>
       </c>
       <c r="G66" s="58">
         <v>2</v>
@@ -9887,7 +9911,7 @@
       </c>
       <c r="I66" s="60">
         <f t="shared" si="39"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J66" s="79"/>
       <c r="K66" s="87"/>
@@ -9946,28 +9970,32 @@
       <c r="BL66" s="87"/>
       <c r="BM66" s="87"/>
       <c r="BN66" s="87"/>
-      <c r="BO66" s="148"/>
-      <c r="BP66" s="148"/>
-      <c r="BQ66" s="148"/>
-      <c r="BR66" s="148"/>
-      <c r="BS66" s="148"/>
+      <c r="BO66" s="149"/>
+      <c r="BP66" s="149"/>
+      <c r="BQ66" s="149"/>
+      <c r="BR66" s="149"/>
+      <c r="BS66" s="149"/>
+      <c r="BW66" s="160"/>
+      <c r="BX66" s="160"/>
+      <c r="BY66" s="160"/>
+      <c r="BZ66" s="160"/>
     </row>
     <row r="67" spans="1:83" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A67" s="56">
-        <v>7.6</v>
+        <v>7.5</v>
       </c>
       <c r="B67" s="106" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C67" s="57" t="s">
         <v>143</v>
       </c>
       <c r="D67" s="107"/>
       <c r="E67" s="82">
-        <v>43927</v>
+        <v>43938</v>
       </c>
       <c r="F67" s="83">
-        <v>43931</v>
+        <v>43942</v>
       </c>
       <c r="G67" s="58">
         <v>2</v>
@@ -9977,7 +10005,7 @@
       </c>
       <c r="I67" s="60">
         <f t="shared" si="39"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J67" s="79"/>
       <c r="K67" s="87"/>
@@ -10036,37 +10064,42 @@
       <c r="BL67" s="87"/>
       <c r="BM67" s="87"/>
       <c r="BN67" s="87"/>
-      <c r="BO67" s="148"/>
-      <c r="BP67" s="148"/>
-      <c r="BQ67" s="148"/>
-      <c r="BR67" s="148"/>
-      <c r="BS67" s="148"/>
-    </row>
-    <row r="68" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="BO67" s="149"/>
+      <c r="BP67" s="149"/>
+      <c r="BQ67" s="149"/>
+      <c r="BR67" s="149"/>
+      <c r="BS67" s="149"/>
+      <c r="BW67" s="160"/>
+      <c r="BX67" s="160"/>
+      <c r="BY67" s="160"/>
+      <c r="BZ67" s="160"/>
+    </row>
+    <row r="68" spans="1:83" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A68" s="56">
-        <v>7.7</v>
+        <v>7.6</v>
       </c>
       <c r="B68" s="106" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="C68" s="57" t="s">
         <v>143</v>
       </c>
       <c r="D68" s="107"/>
       <c r="E68" s="82">
-        <v>43920</v>
+        <v>43939</v>
       </c>
       <c r="F68" s="83">
-        <v>43924</v>
+        <v>43943</v>
       </c>
       <c r="G68" s="58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H68" s="59">
         <v>0</v>
       </c>
       <c r="I68" s="60">
-        <v>5</v>
+        <f t="shared" si="39"/>
+        <v>3</v>
       </c>
       <c r="J68" s="79"/>
       <c r="K68" s="87"/>
@@ -10125,16 +10158,21 @@
       <c r="BL68" s="87"/>
       <c r="BM68" s="87"/>
       <c r="BN68" s="87"/>
-    </row>
-    <row r="69" spans="1:83" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="BO68" s="149"/>
+      <c r="BP68" s="149"/>
+      <c r="BQ68" s="149"/>
+      <c r="BR68" s="149"/>
+      <c r="BS68" s="149"/>
+    </row>
+    <row r="69" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="56">
-        <v>7.8</v>
+        <v>7.7</v>
       </c>
       <c r="B69" s="106" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C69" s="57" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D69" s="107"/>
       <c r="E69" s="82">
@@ -10150,7 +10188,6 @@
         <v>0</v>
       </c>
       <c r="I69" s="60">
-        <f t="shared" ref="I69:I73" si="40">IF(OR(F69=0,E69=0)," - ",NETWORKDAYS(E69,F69))</f>
         <v>5</v>
       </c>
       <c r="J69" s="79"/>
@@ -10211,181 +10248,175 @@
       <c r="BM69" s="87"/>
       <c r="BN69" s="87"/>
     </row>
-    <row r="70" spans="1:83" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A70" s="49" t="str">
+    <row r="70" spans="1:83" s="57" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A70" s="56">
+        <v>7.8</v>
+      </c>
+      <c r="B70" s="106" t="s">
+        <v>154</v>
+      </c>
+      <c r="C70" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D70" s="107"/>
+      <c r="E70" s="82">
+        <v>43920</v>
+      </c>
+      <c r="F70" s="83">
+        <v>43924</v>
+      </c>
+      <c r="G70" s="58">
+        <v>1</v>
+      </c>
+      <c r="H70" s="59">
+        <v>0</v>
+      </c>
+      <c r="I70" s="60">
+        <f t="shared" ref="I70:I74" si="40">IF(OR(F70=0,E70=0)," - ",NETWORKDAYS(E70,F70))</f>
+        <v>5</v>
+      </c>
+      <c r="J70" s="79"/>
+      <c r="K70" s="87"/>
+      <c r="L70" s="87"/>
+      <c r="M70" s="87"/>
+      <c r="N70" s="87"/>
+      <c r="O70" s="87"/>
+      <c r="P70" s="87"/>
+      <c r="Q70" s="87"/>
+      <c r="R70" s="87"/>
+      <c r="S70" s="87"/>
+      <c r="T70" s="87"/>
+      <c r="U70" s="87"/>
+      <c r="V70" s="87"/>
+      <c r="W70" s="87"/>
+      <c r="X70" s="87"/>
+      <c r="Y70" s="87"/>
+      <c r="Z70" s="87"/>
+      <c r="AA70" s="87"/>
+      <c r="AB70" s="87"/>
+      <c r="AC70" s="87"/>
+      <c r="AD70" s="87"/>
+      <c r="AE70" s="87"/>
+      <c r="AF70" s="87"/>
+      <c r="AG70" s="87"/>
+      <c r="AH70" s="87"/>
+      <c r="AI70" s="87"/>
+      <c r="AJ70" s="87"/>
+      <c r="AK70" s="87"/>
+      <c r="AL70" s="87"/>
+      <c r="AM70" s="87"/>
+      <c r="AN70" s="87"/>
+      <c r="AO70" s="87"/>
+      <c r="AP70" s="87"/>
+      <c r="AQ70" s="87"/>
+      <c r="AR70" s="87"/>
+      <c r="AS70" s="87"/>
+      <c r="AT70" s="87"/>
+      <c r="AU70" s="87"/>
+      <c r="AV70" s="87"/>
+      <c r="AW70" s="87"/>
+      <c r="AX70" s="87"/>
+      <c r="AY70" s="87"/>
+      <c r="AZ70" s="87"/>
+      <c r="BA70" s="87"/>
+      <c r="BB70" s="87"/>
+      <c r="BC70" s="87"/>
+      <c r="BD70" s="87"/>
+      <c r="BE70" s="87"/>
+      <c r="BF70" s="87"/>
+      <c r="BG70" s="87"/>
+      <c r="BH70" s="87"/>
+      <c r="BI70" s="87"/>
+      <c r="BJ70" s="87"/>
+      <c r="BK70" s="87"/>
+      <c r="BL70" s="87"/>
+      <c r="BM70" s="87"/>
+      <c r="BN70" s="87"/>
+    </row>
+    <row r="71" spans="1:83" s="51" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="49" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>8</v>
       </c>
-      <c r="B70" s="50" t="s">
-        <v>179</v>
-      </c>
-      <c r="D70" s="52"/>
-      <c r="E70" s="84"/>
-      <c r="F70" s="84" t="str">
-        <f t="shared" ref="F70" si="41">IF(ISBLANK(E70)," - ",IF(G70=0,E70,E70+G70-1))</f>
+      <c r="B71" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="D71" s="52"/>
+      <c r="E71" s="84"/>
+      <c r="F71" s="84" t="str">
+        <f t="shared" ref="F71" si="41">IF(ISBLANK(E71)," - ",IF(G71=0,E71,E71+G71-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G70" s="53"/>
-      <c r="H70" s="54"/>
-      <c r="I70" s="55" t="str">
+      <c r="G71" s="53"/>
+      <c r="H71" s="54"/>
+      <c r="I71" s="55" t="str">
         <f t="shared" si="40"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J70" s="80"/>
-      <c r="K70" s="89"/>
-      <c r="L70" s="89"/>
-      <c r="M70" s="89"/>
-      <c r="N70" s="89"/>
-      <c r="O70" s="89"/>
-      <c r="P70" s="89"/>
-      <c r="Q70" s="89"/>
-      <c r="R70" s="89"/>
-      <c r="S70" s="89"/>
-      <c r="T70" s="89"/>
-      <c r="U70" s="89"/>
-      <c r="V70" s="89"/>
-      <c r="W70" s="89"/>
-      <c r="X70" s="89"/>
-      <c r="Y70" s="89"/>
-      <c r="Z70" s="89"/>
-      <c r="AA70" s="89"/>
-      <c r="AB70" s="89"/>
-      <c r="AC70" s="89"/>
-      <c r="AD70" s="89"/>
-      <c r="AE70" s="89"/>
-      <c r="AF70" s="89"/>
-      <c r="AG70" s="89"/>
-      <c r="AH70" s="89"/>
-      <c r="AI70" s="89"/>
-      <c r="AJ70" s="89"/>
-      <c r="AK70" s="89"/>
-      <c r="AL70" s="89"/>
-      <c r="AM70" s="89"/>
-      <c r="AN70" s="89"/>
-      <c r="AO70" s="89"/>
-      <c r="AP70" s="89"/>
-      <c r="AQ70" s="89"/>
-      <c r="AR70" s="89"/>
-      <c r="AS70" s="89"/>
-      <c r="AT70" s="89"/>
-      <c r="AU70" s="89"/>
-      <c r="AV70" s="89"/>
-      <c r="AW70" s="89"/>
-      <c r="AX70" s="89"/>
-      <c r="AY70" s="89"/>
-      <c r="AZ70" s="89"/>
-      <c r="BA70" s="89"/>
-      <c r="BB70" s="89"/>
-      <c r="BC70" s="89"/>
-      <c r="BD70" s="89"/>
-      <c r="BE70" s="89"/>
-      <c r="BF70" s="89"/>
-      <c r="BG70" s="89"/>
-      <c r="BH70" s="89"/>
-      <c r="BI70" s="89"/>
-      <c r="BJ70" s="89"/>
-      <c r="BK70" s="89"/>
-      <c r="BL70" s="89"/>
-      <c r="BM70" s="89"/>
-      <c r="BN70" s="89"/>
-    </row>
-    <row r="71" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A71" s="56">
-        <v>6.1</v>
-      </c>
-      <c r="B71" s="106" t="s">
-        <v>180</v>
-      </c>
-      <c r="C71" s="57" t="s">
-        <v>163</v>
-      </c>
-      <c r="D71" s="107"/>
-      <c r="E71" s="82">
-        <v>43934</v>
-      </c>
-      <c r="F71" s="83">
-        <v>43940</v>
-      </c>
-      <c r="G71" s="58">
-        <v>5</v>
-      </c>
-      <c r="H71" s="59">
-        <v>0</v>
-      </c>
-      <c r="I71" s="60">
-        <f t="shared" si="40"/>
-        <v>5</v>
-      </c>
-      <c r="J71" s="79"/>
-      <c r="K71" s="87"/>
-      <c r="L71" s="87"/>
-      <c r="M71" s="87"/>
-      <c r="N71" s="87"/>
-      <c r="O71" s="87"/>
-      <c r="P71" s="87"/>
-      <c r="Q71" s="87"/>
-      <c r="R71" s="87"/>
-      <c r="S71" s="87"/>
-      <c r="T71" s="87"/>
-      <c r="U71" s="87"/>
-      <c r="V71" s="87"/>
-      <c r="W71" s="87"/>
-      <c r="X71" s="87"/>
-      <c r="Y71" s="87"/>
-      <c r="Z71" s="87"/>
-      <c r="AA71" s="87"/>
-      <c r="AB71" s="87"/>
-      <c r="AC71" s="87"/>
-      <c r="AD71" s="87"/>
-      <c r="AE71" s="87"/>
-      <c r="AF71" s="87"/>
-      <c r="AG71" s="87"/>
-      <c r="AH71" s="87"/>
-      <c r="AI71" s="87"/>
-      <c r="AJ71" s="87"/>
-      <c r="AK71" s="87"/>
-      <c r="AL71" s="87"/>
-      <c r="AM71" s="87"/>
-      <c r="AN71" s="87"/>
-      <c r="AO71" s="87"/>
-      <c r="AP71" s="87"/>
-      <c r="AQ71" s="87"/>
-      <c r="AR71" s="87"/>
-      <c r="AS71" s="87"/>
-      <c r="AT71" s="87"/>
-      <c r="AU71" s="87"/>
-      <c r="AV71" s="87"/>
-      <c r="AW71" s="87"/>
-      <c r="AX71" s="87"/>
-      <c r="AY71" s="87"/>
-      <c r="AZ71" s="87"/>
-      <c r="BA71" s="87"/>
-      <c r="BB71" s="87"/>
-      <c r="BC71" s="87"/>
-      <c r="BD71" s="87"/>
-      <c r="BE71" s="87"/>
-      <c r="BF71" s="87"/>
-      <c r="BG71" s="87"/>
-      <c r="BH71" s="87"/>
-      <c r="BI71" s="87"/>
-      <c r="BJ71" s="87"/>
-      <c r="BK71" s="87"/>
-      <c r="BL71" s="87"/>
-      <c r="BM71" s="87"/>
-      <c r="BN71" s="87"/>
-      <c r="BV71" s="148"/>
-      <c r="BW71" s="148"/>
-      <c r="BX71" s="148"/>
-      <c r="BY71" s="148"/>
-      <c r="BZ71" s="148"/>
-      <c r="CE71" s="149"/>
+      <c r="J71" s="80"/>
+      <c r="K71" s="89"/>
+      <c r="L71" s="89"/>
+      <c r="M71" s="89"/>
+      <c r="N71" s="89"/>
+      <c r="O71" s="89"/>
+      <c r="P71" s="89"/>
+      <c r="Q71" s="89"/>
+      <c r="R71" s="89"/>
+      <c r="S71" s="89"/>
+      <c r="T71" s="89"/>
+      <c r="U71" s="89"/>
+      <c r="V71" s="89"/>
+      <c r="W71" s="89"/>
+      <c r="X71" s="89"/>
+      <c r="Y71" s="89"/>
+      <c r="Z71" s="89"/>
+      <c r="AA71" s="89"/>
+      <c r="AB71" s="89"/>
+      <c r="AC71" s="89"/>
+      <c r="AD71" s="89"/>
+      <c r="AE71" s="89"/>
+      <c r="AF71" s="89"/>
+      <c r="AG71" s="89"/>
+      <c r="AH71" s="89"/>
+      <c r="AI71" s="89"/>
+      <c r="AJ71" s="89"/>
+      <c r="AK71" s="89"/>
+      <c r="AL71" s="89"/>
+      <c r="AM71" s="89"/>
+      <c r="AN71" s="89"/>
+      <c r="AO71" s="89"/>
+      <c r="AP71" s="89"/>
+      <c r="AQ71" s="89"/>
+      <c r="AR71" s="89"/>
+      <c r="AS71" s="89"/>
+      <c r="AT71" s="89"/>
+      <c r="AU71" s="89"/>
+      <c r="AV71" s="89"/>
+      <c r="AW71" s="89"/>
+      <c r="AX71" s="89"/>
+      <c r="AY71" s="89"/>
+      <c r="AZ71" s="89"/>
+      <c r="BA71" s="89"/>
+      <c r="BB71" s="89"/>
+      <c r="BC71" s="89"/>
+      <c r="BD71" s="89"/>
+      <c r="BE71" s="89"/>
+      <c r="BF71" s="89"/>
+      <c r="BG71" s="89"/>
+      <c r="BH71" s="89"/>
+      <c r="BI71" s="89"/>
+      <c r="BJ71" s="89"/>
+      <c r="BK71" s="89"/>
+      <c r="BL71" s="89"/>
+      <c r="BM71" s="89"/>
+      <c r="BN71" s="89"/>
     </row>
     <row r="72" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="56">
-        <v>6.2</v>
+        <v>6.1</v>
       </c>
       <c r="B72" s="106" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C72" s="57" t="s">
         <v>163</v>
@@ -10473,10 +10504,10 @@
     </row>
     <row r="73" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="56">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
       <c r="B73" s="106" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C73" s="57" t="s">
         <v>163</v>
@@ -10562,20 +10593,34 @@
       <c r="BZ73" s="148"/>
       <c r="CE73" s="149"/>
     </row>
-    <row r="74" spans="1:83" s="66" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A74" s="56"/>
-      <c r="B74" s="61"/>
-      <c r="C74" s="61"/>
-      <c r="D74" s="62"/>
-      <c r="E74" s="85"/>
-      <c r="F74" s="85"/>
-      <c r="G74" s="63"/>
-      <c r="H74" s="64"/>
-      <c r="I74" s="65" t="str">
-        <f t="shared" si="31"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J74" s="81"/>
+    <row r="74" spans="1:83" s="57" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="56">
+        <v>6.3</v>
+      </c>
+      <c r="B74" s="106" t="s">
+        <v>181</v>
+      </c>
+      <c r="C74" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="D74" s="107"/>
+      <c r="E74" s="82">
+        <v>43934</v>
+      </c>
+      <c r="F74" s="83">
+        <v>43940</v>
+      </c>
+      <c r="G74" s="58">
+        <v>5</v>
+      </c>
+      <c r="H74" s="59">
+        <v>0</v>
+      </c>
+      <c r="I74" s="60">
+        <f t="shared" si="40"/>
+        <v>5</v>
+      </c>
+      <c r="J74" s="79"/>
       <c r="K74" s="87"/>
       <c r="L74" s="87"/>
       <c r="M74" s="87"/>
@@ -10632,6 +10677,12 @@
       <c r="BL74" s="87"/>
       <c r="BM74" s="87"/>
       <c r="BN74" s="87"/>
+      <c r="BV74" s="148"/>
+      <c r="BW74" s="148"/>
+      <c r="BX74" s="148"/>
+      <c r="BY74" s="148"/>
+      <c r="BZ74" s="148"/>
+      <c r="CE74" s="149"/>
     </row>
     <row r="75" spans="1:83" s="66" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="56"/>
@@ -10704,15 +10755,89 @@
       <c r="BM75" s="87"/>
       <c r="BN75" s="87"/>
     </row>
+    <row r="76" spans="1:83" s="66" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="56"/>
+      <c r="B76" s="61"/>
+      <c r="C76" s="61"/>
+      <c r="D76" s="62"/>
+      <c r="E76" s="85"/>
+      <c r="F76" s="85"/>
+      <c r="G76" s="63"/>
+      <c r="H76" s="64"/>
+      <c r="I76" s="65" t="str">
+        <f t="shared" si="31"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J76" s="81"/>
+      <c r="K76" s="87"/>
+      <c r="L76" s="87"/>
+      <c r="M76" s="87"/>
+      <c r="N76" s="87"/>
+      <c r="O76" s="87"/>
+      <c r="P76" s="87"/>
+      <c r="Q76" s="87"/>
+      <c r="R76" s="87"/>
+      <c r="S76" s="87"/>
+      <c r="T76" s="87"/>
+      <c r="U76" s="87"/>
+      <c r="V76" s="87"/>
+      <c r="W76" s="87"/>
+      <c r="X76" s="87"/>
+      <c r="Y76" s="87"/>
+      <c r="Z76" s="87"/>
+      <c r="AA76" s="87"/>
+      <c r="AB76" s="87"/>
+      <c r="AC76" s="87"/>
+      <c r="AD76" s="87"/>
+      <c r="AE76" s="87"/>
+      <c r="AF76" s="87"/>
+      <c r="AG76" s="87"/>
+      <c r="AH76" s="87"/>
+      <c r="AI76" s="87"/>
+      <c r="AJ76" s="87"/>
+      <c r="AK76" s="87"/>
+      <c r="AL76" s="87"/>
+      <c r="AM76" s="87"/>
+      <c r="AN76" s="87"/>
+      <c r="AO76" s="87"/>
+      <c r="AP76" s="87"/>
+      <c r="AQ76" s="87"/>
+      <c r="AR76" s="87"/>
+      <c r="AS76" s="87"/>
+      <c r="AT76" s="87"/>
+      <c r="AU76" s="87"/>
+      <c r="AV76" s="87"/>
+      <c r="AW76" s="87"/>
+      <c r="AX76" s="87"/>
+      <c r="AY76" s="87"/>
+      <c r="AZ76" s="87"/>
+      <c r="BA76" s="87"/>
+      <c r="BB76" s="87"/>
+      <c r="BC76" s="87"/>
+      <c r="BD76" s="87"/>
+      <c r="BE76" s="87"/>
+      <c r="BF76" s="87"/>
+      <c r="BG76" s="87"/>
+      <c r="BH76" s="87"/>
+      <c r="BI76" s="87"/>
+      <c r="BJ76" s="87"/>
+      <c r="BK76" s="87"/>
+      <c r="BL76" s="87"/>
+      <c r="BM76" s="87"/>
+      <c r="BN76" s="87"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="25">
-    <mergeCell ref="BV5:CB5"/>
-    <mergeCell ref="CC5:CI5"/>
-    <mergeCell ref="BO4:BU4"/>
-    <mergeCell ref="BO5:BU5"/>
-    <mergeCell ref="BV4:CB4"/>
-    <mergeCell ref="CC4:CI4"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -10723,18 +10848,15 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
+    <mergeCell ref="BV5:CB5"/>
+    <mergeCell ref="CC5:CI5"/>
+    <mergeCell ref="BO4:BU4"/>
+    <mergeCell ref="BO5:BU5"/>
+    <mergeCell ref="BV4:CB4"/>
+    <mergeCell ref="CC4:CI4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H74:H75 H8:H60">
+  <conditionalFormatting sqref="H75:H76 H8:H61">
     <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -10753,7 +10875,7 @@
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN75">
+  <conditionalFormatting sqref="K8:BN76">
     <cfRule type="expression" dxfId="5" priority="68">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
@@ -10761,12 +10883,12 @@
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K74:BN75 BO6:CI7 K6:BN60">
+  <conditionalFormatting sqref="K75:BN76 BO6:CI7 K6:BN61">
     <cfRule type="expression" dxfId="3" priority="28">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H61:H68">
+  <conditionalFormatting sqref="H62:H69">
     <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -10780,12 +10902,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K61:BN68">
+  <conditionalFormatting sqref="K62:BN69">
     <cfRule type="expression" dxfId="2" priority="14">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H69">
+  <conditionalFormatting sqref="H70">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -10799,12 +10921,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K69:BN69">
+  <conditionalFormatting sqref="K70:BN70">
     <cfRule type="expression" dxfId="1" priority="10">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H70:H73">
+  <conditionalFormatting sqref="H71:H74">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -10818,7 +10940,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K70:BN73">
+  <conditionalFormatting sqref="K71:BN74">
     <cfRule type="expression" dxfId="0" priority="6">
       <formula>K$6=TODAY()</formula>
     </cfRule>
@@ -10833,7 +10955,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A75:B75 E16 E33 E42 E74:H75 G16:H16 G33:H33 G42:H42 H39 G45:H45 H43:H44 A74" unlockedFormula="1"/>
+    <ignoredError sqref="H9 A76:B76 E16 E33 E42 E75:H76 G16:H16 G33:H33 G42:H42 G45 A75" unlockedFormula="1"/>
     <ignoredError sqref="A42 A33 A16" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
@@ -10882,7 +11004,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H74:H75 H8:H60</xm:sqref>
+          <xm:sqref>H75:H76 H8:H61</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0F99DC93-F37E-44FD-BA80-440E3A4D599D}">
@@ -10897,7 +11019,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H61:H68</xm:sqref>
+          <xm:sqref>H62:H69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B9031F11-912A-4A5C-85BD-BFB059CEAD5B}">
@@ -10912,7 +11034,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H69</xm:sqref>
+          <xm:sqref>H70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{437A52F8-D2E6-4093-9466-950C3C255C94}">
@@ -10927,7 +11049,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H70:H73</xm:sqref>
+          <xm:sqref>H71:H74</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>